<commit_message>
Updata xlsx file for ED and BR filtration
</commit_message>
<xml_diff>
--- a/Data/ED_and_BR_work_together_in_all_samples.xlsx
+++ b/Data/ED_and_BR_work_together_in_all_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maria\IB\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B70607-848B-48C5-A22D-D6C676E99F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1181B6FF-FCF5-42B3-A2B6-1F5F45EB4650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>OverAll_CB</t>
   </si>
   <si>
-    <t>filtered_by_BR</t>
-  </si>
-  <si>
     <t>BR_yes_ED_yes</t>
   </si>
   <si>
@@ -70,6 +67,15 @@
   </si>
   <si>
     <t>knee_point</t>
+  </si>
+  <si>
+    <t>filtered_by_BR(inflection)</t>
+  </si>
+  <si>
+    <t>filtered_by_ED</t>
+  </si>
+  <si>
+    <t>Summ</t>
   </si>
 </sst>
 </file>
@@ -420,15 +426,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -456,11 +463,14 @@
       <c r="I1">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
       <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -500,7 +510,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>921</v>
@@ -535,7 +545,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>409</v>
@@ -570,7 +580,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>6487</v>
@@ -599,7 +609,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>97</v>
@@ -628,7 +638,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>1418</v>
@@ -655,9 +665,9 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>8486</v>
@@ -684,117 +694,154 @@
         <v>3980</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>6079</v>
+      </c>
+      <c r="C9">
+        <v>4673</v>
+      </c>
+      <c r="D9">
+        <v>12540</v>
+      </c>
+      <c r="E9">
+        <v>7207</v>
+      </c>
+      <c r="F9">
+        <v>4413</v>
+      </c>
+      <c r="G9">
+        <v>2812</v>
+      </c>
+      <c r="H9">
+        <v>7302</v>
+      </c>
+      <c r="I9">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>3168</v>
+      </c>
+      <c r="C10">
+        <v>2641</v>
+      </c>
+      <c r="D10">
+        <v>1849</v>
+      </c>
+      <c r="E10">
+        <v>1186</v>
+      </c>
+      <c r="F10">
+        <v>3047</v>
+      </c>
+      <c r="G10">
+        <v>2477</v>
+      </c>
+      <c r="H10">
+        <v>1894</v>
+      </c>
+      <c r="I10">
+        <v>1299</v>
+      </c>
+      <c r="K10">
+        <v>888</v>
+      </c>
+      <c r="L10">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9">
-        <v>3168</v>
-      </c>
-      <c r="C9">
-        <v>2641</v>
-      </c>
-      <c r="D9">
-        <v>1849</v>
-      </c>
-      <c r="E9">
-        <v>1186</v>
-      </c>
-      <c r="F9">
-        <v>3047</v>
-      </c>
-      <c r="G9">
-        <v>2477</v>
-      </c>
-      <c r="H9">
-        <v>1894</v>
-      </c>
-      <c r="I9">
-        <v>1299</v>
-      </c>
-      <c r="K9">
-        <v>888</v>
-      </c>
-      <c r="L9">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="1">
+        <v>2737</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2265</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1848</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1146</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2484</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2037</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1644</v>
+      </c>
+      <c r="I11" s="1">
+        <v>610</v>
+      </c>
+      <c r="J11">
+        <f>SUM(B11:I11)</f>
+        <v>14771</v>
+      </c>
+      <c r="K11" s="1">
+        <v>768</v>
+      </c>
+      <c r="L11" s="1">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
-        <v>2737</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2265</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1848</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1146</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="B12" s="2">
+        <f xml:space="preserve"> B10 - B11</f>
         <v>431</v>
       </c>
-      <c r="G10" s="1">
-        <v>623</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1644</v>
-      </c>
-      <c r="I10" s="1">
-        <v>610</v>
-      </c>
-      <c r="K10" s="1">
-        <v>765</v>
-      </c>
-      <c r="L10" s="1">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2">
-        <f xml:space="preserve"> B9 - B10</f>
-        <v>431</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" ref="C11:I11" si="0" xml:space="preserve"> C9 - C10</f>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:I12" si="0" xml:space="preserve"> C10 - C11</f>
         <v>376</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>2616</v>
-      </c>
-      <c r="G11" s="2">
+        <v>563</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>1854</v>
-      </c>
-      <c r="H11" s="2">
+        <v>440</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>689</v>
       </c>
-      <c r="K11" s="2">
-        <v>123</v>
-      </c>
-      <c r="L11" s="2">
-        <v>271</v>
+      <c r="J12" s="2">
+        <f>SUM(B12:I12)</f>
+        <v>2790</v>
+      </c>
+      <c r="K12" s="2">
+        <v>120</v>
+      </c>
+      <c r="L12" s="2">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update xlsx file, add analysis in (knee, inflection) range
</commit_message>
<xml_diff>
--- a/Data/ED_and_BR_work_together_in_all_samples.xlsx
+++ b/Data/ED_and_BR_work_together_in_all_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maria\IB\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1181B6FF-FCF5-42B3-A2B6-1F5F45EB4650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60809A0-4A5B-4D07-BD27-CBDE1380245C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>OverAll_CB</t>
   </si>
   <si>
-    <t>BR_yes_ED_yes</t>
-  </si>
-  <si>
-    <t>BR_yes_ED_no</t>
-  </si>
-  <si>
     <t>inflection_point</t>
   </si>
   <si>
@@ -69,20 +63,38 @@
     <t>knee_point</t>
   </si>
   <si>
+    <t xml:space="preserve">суммарный </t>
+  </si>
+  <si>
     <t>filtered_by_BR(inflection)</t>
   </si>
   <si>
     <t>filtered_by_ED</t>
   </si>
   <si>
-    <t>Summ</t>
+    <t>ED_yes in (inflection, knee)</t>
+  </si>
+  <si>
+    <t>ED_no in (inflection, knee)</t>
+  </si>
+  <si>
+    <t>BR_yes_ED_yes &gt;inflection</t>
+  </si>
+  <si>
+    <t>BR_yes_ED_no &gt;inflection</t>
+  </si>
+  <si>
+    <t>yes/all &gt; inflection</t>
+  </si>
+  <si>
+    <t>all in (inflection, knee)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +114,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -140,10 +166,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -426,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
     <col min="10" max="10" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -464,13 +500,13 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -510,7 +546,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>921</v>
@@ -545,7 +581,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>409</v>
@@ -580,7 +616,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>6487</v>
@@ -609,7 +645,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>97</v>
@@ -638,7 +674,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>1418</v>
@@ -667,7 +703,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>8486</v>
@@ -696,7 +732,7 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>6079</v>
@@ -725,7 +761,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>3168</v>
@@ -751,6 +787,10 @@
       <c r="I10">
         <v>1299</v>
       </c>
+      <c r="J10">
+        <f xml:space="preserve"> J11 +J12</f>
+        <v>17561</v>
+      </c>
       <c r="K10">
         <v>888</v>
       </c>
@@ -760,7 +800,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
         <v>2737</v>
@@ -799,7 +839,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
         <f xml:space="preserve"> B10 - B11</f>
@@ -844,7 +884,115 @@
         <v>270</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <f>B11/B10</f>
+        <v>0.86395202020202022</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:J13" si="1">C11/C10</f>
+        <v>0.85762968572510412</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>0.99945916711736071</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.96627318718381117</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.81522809320643252</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.82236576503835279</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.86800422386483633</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0.46959199384141648</v>
+      </c>
+      <c r="J13">
+        <f>J11/J10</f>
+        <v>0.84112522065941575</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <v>176</v>
+      </c>
+      <c r="C15">
+        <v>71</v>
+      </c>
+      <c r="D15">
+        <v>267</v>
+      </c>
+      <c r="E15">
+        <v>326</v>
+      </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>379</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
+        <v>607</v>
+      </c>
+      <c r="C17" s="6">
+        <v>444</v>
+      </c>
+      <c r="D17" s="5">
+        <v>268</v>
+      </c>
+      <c r="E17" s="6">
+        <v>366</v>
+      </c>
+      <c r="F17" s="5">
+        <v>586</v>
+      </c>
+      <c r="G17" s="6">
+        <v>453</v>
+      </c>
+      <c r="H17" s="5">
+        <v>625</v>
+      </c>
+      <c r="I17" s="6">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>